<commit_message>
Cuadruplos de expressiones 100% funcionando
Se trabajo en cuadruplos de:
incremento
asignacion
print

Tambien ya pueden ir constantes en los cuadruplos
</commit_message>
<xml_diff>
--- a/Memoria Virtual.xlsx
+++ b/Memoria Virtual.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Memoria Global</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>En la memoria local se resetea el index cuando la funcion muere</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -246,19 +249,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color rgb="FFFF0000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -363,6 +353,26 @@
       <bottom style="double">
         <color theme="5" tint="0.39997558519241921"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -370,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -381,25 +391,27 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -716,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:N38"/>
+  <dimension ref="C1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,170 +817,233 @@
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="6"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="5">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5">
+        <v>18001</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="6"/>
+      <c r="G13" s="5">
         <v>20000</v>
       </c>
     </row>
-    <row r="11" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="13" t="s">
+    <row r="14" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G14" s="5">
         <v>20001</v>
-      </c>
-    </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="F12" s="14"/>
-      <c r="N12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="15"/>
-      <c r="G13" s="5">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="14" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="5">
-        <v>23001</v>
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F15" s="14"/>
+      <c r="N15" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F16" s="15"/>
       <c r="G16" s="5">
-        <v>26000</v>
+        <v>23000</v>
       </c>
     </row>
     <row r="17" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="14" t="s">
-        <v>6</v>
+      <c r="F17" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="G17" s="5">
-        <v>26001</v>
+        <v>23001</v>
       </c>
     </row>
     <row r="18" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F18" s="14"/>
     </row>
     <row r="19" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="14"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="5">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="20" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="5">
+        <v>26001</v>
+      </c>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="15"/>
+      <c r="G22" s="5">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="23" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="5">
+        <v>28001</v>
+      </c>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F24" s="14"/>
+    </row>
+    <row r="25" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="14"/>
+      <c r="G25" s="5">
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="17" t="s">
+    <row r="26" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G26" s="5">
         <v>30001</v>
-      </c>
-    </row>
-    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="19"/>
-      <c r="G22" s="5">
-        <v>33000</v>
-      </c>
-      <c r="K22" s="20"/>
-    </row>
-    <row r="23" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="5">
-        <v>33001</v>
-      </c>
-    </row>
-    <row r="24" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F24" s="18"/>
-    </row>
-    <row r="25" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="19"/>
-      <c r="G25" s="5">
-        <v>36000</v>
-      </c>
-    </row>
-    <row r="26" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G26" s="5">
-        <v>36001</v>
       </c>
     </row>
     <row r="27" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="18"/>
+      <c r="F28" s="19"/>
       <c r="G28" s="5">
+        <v>33000</v>
+      </c>
+      <c r="K28" s="20"/>
+    </row>
+    <row r="29" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="5">
+        <v>33001</v>
+      </c>
+    </row>
+    <row r="30" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="19"/>
+      <c r="G31" s="5">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="32" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="5">
+        <v>36001</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="19"/>
+      <c r="G34" s="5">
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="5">
+        <v>38001</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="18"/>
+      <c r="G37" s="5">
         <v>40000</v>
       </c>
     </row>
-    <row r="29" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="22" t="s">
+    <row r="38" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G38" s="5">
         <v>40001</v>
       </c>
     </row>
-    <row r="30" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="F30" s="23"/>
-    </row>
-    <row r="31" spans="6:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="24"/>
-      <c r="G31" s="5">
-        <v>43000</v>
-      </c>
-    </row>
-    <row r="32" spans="6:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F32" s="25" t="s">
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="23"/>
+    </row>
+    <row r="40" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="24"/>
+      <c r="G40" s="5">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F41" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="5">
-        <v>43001</v>
-      </c>
-    </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F33" s="23"/>
-    </row>
-    <row r="34" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="24"/>
-      <c r="G34" s="5">
-        <v>46000</v>
-      </c>
-    </row>
-    <row r="35" spans="6:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="F35" s="23" t="s">
+      <c r="G41" s="5">
+        <v>44001</v>
+      </c>
+    </row>
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F42" s="23"/>
+    </row>
+    <row r="43" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="24"/>
+      <c r="G43" s="5">
+        <v>47000</v>
+      </c>
+    </row>
+    <row r="44" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G35" s="5">
-        <v>46001</v>
-      </c>
-    </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F36" s="23"/>
-    </row>
-    <row r="37" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="26"/>
-      <c r="G37" s="5">
+      <c r="G44" s="27">
+        <v>47001</v>
+      </c>
+    </row>
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+    </row>
+    <row r="46" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F46" s="24"/>
+      <c r="G46" s="5">
         <v>50000</v>
       </c>
-      <c r="H37" s="27"/>
-    </row>
-    <row r="38" spans="6:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="47" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F50" s="29"/>
+      <c r="G50" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="K1:N1"/>

</xml_diff>

<commit_message>
Eliminacion de asignaciones en definiciones de vars
Ya no se puede asignar un valor al momento de definir una variable.

Todos los valores ya aparecen en la tabla de constantes ya que se agrego los booleanos tmbn.

Tmbn se completo la functionDir para main y global. (Agregandole su cuadruplo donde empieza, la cantidad de parametros y cantidad de variables)
</commit_message>
<xml_diff>
--- a/Memoria Virtual.xlsx
+++ b/Memoria Virtual.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
   <si>
     <t>Memoria Global</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t>Boolean</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -373,6 +376,17 @@
         <color theme="5" tint="0.39997558519241921"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -380,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -413,6 +427,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -730,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +1008,7 @@
     <row r="40" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F40" s="24"/>
       <c r="G40" s="5">
-        <v>44000</v>
+        <v>43000</v>
       </c>
     </row>
     <row r="41" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1001,7 +1016,7 @@
         <v>5</v>
       </c>
       <c r="G41" s="5">
-        <v>44001</v>
+        <v>43001</v>
       </c>
     </row>
     <row r="42" spans="6:7" x14ac:dyDescent="0.25">
@@ -1010,7 +1025,7 @@
     <row r="43" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F43" s="24"/>
       <c r="G43" s="5">
-        <v>47000</v>
+        <v>46000</v>
       </c>
     </row>
     <row r="44" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1018,31 +1033,39 @@
         <v>6</v>
       </c>
       <c r="G44" s="27">
-        <v>47001</v>
+        <v>46001</v>
       </c>
     </row>
     <row r="45" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F46" s="24"/>
       <c r="G46" s="5">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="47" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="27">
+        <v>48001</v>
+      </c>
+    </row>
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F48" s="28"/>
+      <c r="G48" s="27"/>
+    </row>
+    <row r="49" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F49" s="30"/>
+      <c r="G49" s="27">
         <v>50000</v>
       </c>
     </row>
-    <row r="47" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="F50" s="29"/>
-      <c r="G50" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>